<commit_message>
risolto bug delle features più importanti
</commit_message>
<xml_diff>
--- a/most_important_features.xlsx
+++ b/most_important_features.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,866 +436,1030 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Features</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>LogisticRegression</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>SVM</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>RandomForest</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Aminooctanoic acid</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>-0.02483805884368494</v>
-      </c>
       <c r="C2" t="n">
-        <v>-0.009252539184085591</v>
+        <v>0.03251645521797115</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01982665510159755</v>
+        <v>0.02552968423754527</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.01128666146299334</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Androsterone sulfate</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>-0.01681577773226414</v>
-      </c>
       <c r="C3" t="n">
-        <v>-0.01906375423963125</v>
+        <v>0.03266129202105161</v>
       </c>
       <c r="D3" t="n">
-        <v>0.100106816678693</v>
+        <v>0.02391229659686182</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.008591896860457615</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Arachidonic acid</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>-0.0093722047813832</v>
-      </c>
       <c r="C4" t="n">
-        <v>-0.005738837271187534</v>
+        <v>0.0384779323693528</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.01829296779780096</v>
+        <v>0.02973725661164587</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.01530773690105945</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Arginine</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>-0.03128594594771577</v>
-      </c>
       <c r="C5" t="n">
-        <v>-0.01706106711018943</v>
+        <v>0.02088643850539617</v>
       </c>
       <c r="D5" t="n">
-        <v>0.03734497545459931</v>
+        <v>0.01569368114886248</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.006171595617626538</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Asymmetric dimethylarginine</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>0.01301155487805269</v>
-      </c>
       <c r="C6" t="n">
-        <v>0.01579938498351105</v>
+        <v>0.02514955138505637</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.1465319002355802</v>
+        <v>0.02567198908860041</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.01116489886903217</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Bilirubin</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>0.02378971017000647</v>
-      </c>
       <c r="C7" t="n">
-        <v>0.01679702651097705</v>
+        <v>0.02680258398394172</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.07458825272229799</v>
+        <v>0.02118017450963643</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.008496609057637673</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Biliverdin</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>0.0198551767559354</v>
-      </c>
       <c r="C8" t="n">
-        <v>0.007955397086433454</v>
+        <v>0.03741173321285227</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1583863215322834</v>
+        <v>0.02875984318681762</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.01356319270779244</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>CAR 10:0</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>0.01624602571949997</v>
-      </c>
       <c r="C9" t="n">
-        <v>0.02151841915361247</v>
+        <v>0.04521143369260198</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1175506399132085</v>
+        <v>0.02920013367599956</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.01886036034288465</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>CAR 10:1</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>0.03537271097869003</v>
-      </c>
       <c r="C10" t="n">
-        <v>0.02913853532169876</v>
+        <v>0.044047741663561</v>
       </c>
       <c r="D10" t="n">
-        <v>0.111135807350785</v>
+        <v>0.02935024982135654</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.01860521358734116</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>CAR 14:1</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>0.004008284869220961</v>
-      </c>
       <c r="C11" t="n">
-        <v>-0.002217959155760903</v>
+        <v>0.02307749637555451</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.07830519653164958</v>
+        <v>0.02426181198294153</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.008388999187357835</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>CAR 16:1_A</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>-0.01084003083577647</v>
-      </c>
       <c r="C12" t="n">
-        <v>-0.02289562242879174</v>
+        <v>0.02237589379141718</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.100426046696388</v>
+        <v>0.02325585598827717</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.007790031424879489</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>CAR 16:1_B</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>-0.03797335323008783</v>
-      </c>
       <c r="C13" t="n">
-        <v>-0.02192775156031267</v>
+        <v>0.02213396682135894</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.1193528170855471</v>
+        <v>0.02192356239442436</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.00912541643177887</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>CAR 16:2</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>-0.008262405817287133</v>
-      </c>
       <c r="C14" t="n">
-        <v>-0.01312644090913843</v>
+        <v>0.01932247591288955</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.1105772508777178</v>
+        <v>0.02171120465338061</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.00833772481887458</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>CAR 18:1_A</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>-0.01440683061623436</v>
-      </c>
       <c r="C15" t="n">
-        <v>-0.02293219319910024</v>
+        <v>0.02704305544951774</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.1157579217840598</v>
+        <v>0.02494942763931513</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.00897825640550763</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>CAR 18:1_B</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>-0.01161922785419429</v>
-      </c>
       <c r="C16" t="n">
-        <v>-0.04921592092223927</v>
+        <v>0.01708176104884212</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.08367179076805341</v>
+        <v>0.02050837179521456</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.005982311593021731</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>CAR 2:0</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>-0.02337524147851432</v>
-      </c>
       <c r="C17" t="n">
-        <v>-0.03049920454022123</v>
+        <v>0.0213244098893862</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.1411062786786791</v>
+        <v>0.02463640795075801</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.009520532427183311</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>CAR 3:0</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>-0.03256908145914318</v>
-      </c>
       <c r="C18" t="n">
-        <v>-0.04097867887638859</v>
+        <v>0.01505469431839282</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.04368133010238451</v>
+        <v>0.01670306631840935</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.005103707017751656</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>CAR 4:0</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>-0.02110897187918596</v>
-      </c>
       <c r="C19" t="n">
-        <v>-0.01955227843506186</v>
+        <v>0.0280400590239025</v>
       </c>
       <c r="D19" t="n">
-        <v>0.01210389967253519</v>
+        <v>0.02295999348428169</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.008995696801506411</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>CAR 5:0</t>
         </is>
       </c>
-      <c r="B20" t="n">
-        <v>0.01253866472480419</v>
-      </c>
       <c r="C20" t="n">
-        <v>-0.001372020579334849</v>
+        <v>0.01140171254685675</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.04751461896437165</v>
+        <v>0.01419096049305987</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.004549412795270165</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="inlineStr">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>CAR 5:1;O2</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>-0.05735785797180228</v>
-      </c>
       <c r="C21" t="n">
-        <v>-0.04195737377723845</v>
+        <v>0.02135635251137514</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.1127580699914199</v>
+        <v>0.02315436608558357</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.008750362553488156</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>CAR 5:1</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>0.04395276126316437</v>
-      </c>
       <c r="C22" t="n">
-        <v>0.02923432431088283</v>
+        <v>0.01872807972175164</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.05910959123872592</v>
+        <v>0.01948989641024755</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.005886693295396023</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>CAR 6:0</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>0.001319897253771047</v>
-      </c>
       <c r="C23" t="n">
-        <v>-0.008857068322373741</v>
+        <v>0.03866768347261354</v>
       </c>
       <c r="D23" t="n">
-        <v>0.01011440822731301</v>
+        <v>0.03049098284154712</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.0162023486807887</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>CAR 8:0</t>
         </is>
       </c>
-      <c r="B24" t="n">
-        <v>0.00982550473740299</v>
-      </c>
       <c r="C24" t="n">
-        <v>0.005162270120128883</v>
+        <v>0.04484209128774547</v>
       </c>
       <c r="D24" t="n">
-        <v>0.1058822531589594</v>
+        <v>0.03004829286237612</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.01849367851823286</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>CAR 8:1</t>
         </is>
       </c>
-      <c r="B25" t="n">
-        <v>-0.0048858333754635</v>
-      </c>
       <c r="C25" t="n">
-        <v>0.01181141271950405</v>
+        <v>0.01883737014034351</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.02309679422524737</v>
+        <v>0.01842984229263323</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.006965315020625745</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="inlineStr">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>CAR 9:0</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>0.08496945014802786</v>
-      </c>
       <c r="C26" t="n">
-        <v>0.0742634297535547</v>
+        <v>0.03741161022610905</v>
       </c>
       <c r="D26" t="n">
-        <v>0.1217329968966619</v>
+        <v>0.0228929302274579</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.01332931625281685</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="inlineStr">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
         <is>
           <t>Carnitine</t>
         </is>
       </c>
-      <c r="B27" t="n">
-        <v>-0.0220059252022001</v>
-      </c>
       <c r="C27" t="n">
-        <v>-0.02358305817266071</v>
+        <v>0.01227433072170022</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.06110789851961591</v>
+        <v>0.01473564824442825</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.004826728731355862</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="inlineStr">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
         <is>
           <t>Cresol sulfate</t>
         </is>
       </c>
-      <c r="B28" t="n">
-        <v>0.02622799598316532</v>
-      </c>
       <c r="C28" t="n">
-        <v>0.01086674424872971</v>
+        <v>0.03256569208669819</v>
       </c>
       <c r="D28" t="n">
-        <v>0.1189450817266818</v>
+        <v>0.02319941923708428</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.01248801907206423</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="inlineStr">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
         <is>
           <t>Dehydroepiandrosterone sulfate</t>
         </is>
       </c>
-      <c r="B29" t="n">
-        <v>-0.002963805660476729</v>
-      </c>
       <c r="C29" t="n">
-        <v>0.007950904511602621</v>
+        <v>0.03424823089552293</v>
       </c>
       <c r="D29" t="n">
-        <v>0.09560279358947024</v>
+        <v>0.02338696060858632</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.008825755536895262</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="inlineStr">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
         <is>
           <t>Deoxycholic acid glycine conjugate</t>
         </is>
       </c>
-      <c r="B30" t="n">
-        <v>-0.001276613723741598</v>
-      </c>
       <c r="C30" t="n">
-        <v>0.01306646183491796</v>
+        <v>0.03317802722721828</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.1296968451263732</v>
+        <v>0.02683395636882911</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.01172250079250785</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="inlineStr">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t xml:space="preserve">Dodecenoylcarnitine </t>
         </is>
       </c>
-      <c r="B31" t="n">
-        <v>0.02635148619485323</v>
-      </c>
       <c r="C31" t="n">
-        <v>0.03440787909678492</v>
+        <v>0.0297899522842901</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.04005624184419936</v>
+        <v>0.02701814536555655</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.01073729320668053</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="inlineStr">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
         <is>
           <t>FA 18:1+1O</t>
         </is>
       </c>
-      <c r="B32" t="n">
-        <v>0.008972581870708469</v>
-      </c>
       <c r="C32" t="n">
-        <v>-0.003797341777002894</v>
+        <v>0.03629072498130805</v>
       </c>
       <c r="D32" t="n">
-        <v>0.01552069612501519</v>
+        <v>0.03021689158393082</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.01530834356804905</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="inlineStr">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
         <is>
           <t>Glycerophosphocholine</t>
         </is>
       </c>
-      <c r="B33" t="n">
-        <v>0.0100924669198439</v>
-      </c>
       <c r="C33" t="n">
-        <v>0.01418262434207874</v>
+        <v>0.03620476572724979</v>
       </c>
       <c r="D33" t="n">
-        <v>0.0227890871231064</v>
+        <v>0.0305336852406256</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.0156736496132356</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="inlineStr">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
         <is>
           <t>Histidine</t>
         </is>
       </c>
-      <c r="B34" t="n">
-        <v>0.02576904546043486</v>
-      </c>
       <c r="C34" t="n">
-        <v>0.01549617661046509</v>
+        <v>0.01731087074135054</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.05613091753339475</v>
+        <v>0.01667590341153922</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.006086627178276309</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="inlineStr">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
         <is>
           <t>Homoarginine</t>
         </is>
       </c>
-      <c r="B35" t="n">
-        <v>0.004991613852154883</v>
-      </c>
       <c r="C35" t="n">
-        <v>0.008614522379606136</v>
+        <v>0.02056173882663604</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.03573178074579508</v>
+        <v>0.01969335043916126</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.006074791388355087</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="inlineStr">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
         <is>
           <t>Hydroperoxylinoleic acid</t>
         </is>
       </c>
-      <c r="B36" t="n">
-        <v>-0.06751843607437563</v>
-      </c>
       <c r="C36" t="n">
-        <v>-0.06827081467299782</v>
+        <v>0.02184159913721007</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.1125770536967572</v>
+        <v>0.02394260290926439</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.008610119011599898</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="inlineStr">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>Hydroxyanthranilic acid</t>
         </is>
       </c>
-      <c r="B37" t="n">
-        <v>0.02124749832466974</v>
-      </c>
       <c r="C37" t="n">
-        <v>0.02472063119633727</v>
+        <v>0.03526709657607886</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.1834798775835397</v>
+        <v>0.02880645056156423</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.01513657103689796</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="inlineStr">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>Hydroxypregnenolone sulfate</t>
         </is>
       </c>
-      <c r="B38" t="n">
-        <v>-0.0583693019646358</v>
-      </c>
       <c r="C38" t="n">
-        <v>-0.03323893599817771</v>
+        <v>0.02493063256774879</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.05381661884597153</v>
+        <v>0.02205818202194236</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.005279252443952916</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="inlineStr">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
         <is>
           <t>INDOLE-ACETALDEHYDE</t>
         </is>
       </c>
-      <c r="B39" t="n">
-        <v>-0.01928535034346538</v>
-      </c>
       <c r="C39" t="n">
-        <v>-0.02606947880850439</v>
+        <v>0.01026954964108243</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.009546047598051961</v>
+        <v>0.01161528727224294</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.002565149185691055</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="inlineStr">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
         <is>
           <t>Indoxyl sulfate</t>
         </is>
       </c>
-      <c r="B40" t="n">
-        <v>-0.002009617803669298</v>
-      </c>
       <c r="C40" t="n">
-        <v>0.0102171981623037</v>
+        <v>0.03534572308405757</v>
       </c>
       <c r="D40" t="n">
-        <v>0.1655116386935099</v>
+        <v>0.02537941130430152</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.01445376500723918</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="inlineStr">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
         <is>
           <t>Isoleucylproline</t>
         </is>
       </c>
-      <c r="B41" t="n">
-        <v>0.01210266010708769</v>
-      </c>
       <c r="C41" t="n">
-        <v>0.01390261703352519</v>
+        <v>0.02382415662500156</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.1050030676179055</v>
+        <v>0.02209750381664966</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.009386704052276948</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="inlineStr">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
         <is>
           <t>Methylguanine</t>
         </is>
       </c>
-      <c r="B42" t="n">
-        <v>-0.03692314337631369</v>
-      </c>
       <c r="C42" t="n">
-        <v>-0.01406027778518387</v>
+        <v>0.02412603246652833</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.1186844256086188</v>
+        <v>0.02374852367234388</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.01009804833331819</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="inlineStr">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
         <is>
           <t>Methylhistidine</t>
         </is>
       </c>
-      <c r="B43" t="n">
-        <v>0.01749957009911486</v>
-      </c>
       <c r="C43" t="n">
-        <v>0.002043792111665942</v>
+        <v>0.01654685568912317</v>
       </c>
       <c r="D43" t="n">
-        <v>0.007878296741954999</v>
+        <v>0.01466097132598322</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.002995356342432846</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="inlineStr">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
         <is>
           <t>Methylpyridonecarboxamide</t>
         </is>
       </c>
-      <c r="B44" t="n">
-        <v>0.02800659152765727</v>
-      </c>
       <c r="C44" t="n">
-        <v>0.03384854830598884</v>
+        <v>0.03743188939025789</v>
       </c>
       <c r="D44" t="n">
-        <v>-0.1962975071019802</v>
+        <v>0.03026055610412458</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.0159030304573506</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="inlineStr">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
         <is>
           <t>Paraxanthine</t>
         </is>
       </c>
-      <c r="B45" t="n">
-        <v>0.01762955683704857</v>
-      </c>
       <c r="C45" t="n">
-        <v>0.00840352681365401</v>
+        <v>0.03073902846952543</v>
       </c>
       <c r="D45" t="n">
-        <v>0.05694129550189168</v>
+        <v>0.02274174515426732</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.009552196459849959</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="inlineStr">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
         <is>
           <t>Phenylacetylglutamine</t>
         </is>
       </c>
-      <c r="B46" t="n">
-        <v>0.005438706652296917</v>
-      </c>
       <c r="C46" t="n">
-        <v>0.02848650599636516</v>
+        <v>0.02995374408739871</v>
       </c>
       <c r="D46" t="n">
-        <v>0.07372526358116403</v>
+        <v>0.02014306459832111</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.008794282212872203</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="inlineStr">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
         <is>
           <t>Pregnenolone sulfate</t>
         </is>
       </c>
-      <c r="B47" t="n">
-        <v>-0.04107833406181274</v>
-      </c>
       <c r="C47" t="n">
-        <v>-0.04957149471929633</v>
+        <v>0.03490197133843353</v>
       </c>
       <c r="D47" t="n">
-        <v>-0.1210852829165444</v>
+        <v>0.02607828291613866</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.01034245918270243</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="inlineStr">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
         <is>
           <t>Proline betaine</t>
         </is>
       </c>
-      <c r="B48" t="n">
-        <v>0.0221713955860687</v>
-      </c>
       <c r="C48" t="n">
-        <v>0.02681582046504073</v>
+        <v>0.02017067715272118</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.03889534501078901</v>
+        <v>0.01746400352878342</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.00504079008260697</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="inlineStr">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
         <is>
           <t>Proline-hydroxyproline</t>
         </is>
       </c>
-      <c r="B49" t="n">
-        <v>-0.009654940317774236</v>
-      </c>
       <c r="C49" t="n">
-        <v>-0.005903136008522765</v>
+        <v>0.02063356176287957</v>
       </c>
       <c r="D49" t="n">
-        <v>-0.07830175385198415</v>
+        <v>0.02117236362077514</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.005798272908423874</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="inlineStr">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
         <is>
           <t>Pseudouridine</t>
         </is>
       </c>
-      <c r="B50" t="n">
-        <v>-0.03092142501189152</v>
-      </c>
       <c r="C50" t="n">
-        <v>-0.0203815247089254</v>
+        <v>0.02910541200479706</v>
       </c>
       <c r="D50" t="n">
-        <v>-0.1423710168951116</v>
+        <v>0.02598996127482945</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.01168900135602216</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="inlineStr">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
         <is>
           <t>Sphingosine 1-phosphate</t>
         </is>
       </c>
-      <c r="B51" t="n">
-        <v>-0.04961118480312918</v>
-      </c>
       <c r="C51" t="n">
-        <v>-0.07548700219130333</v>
+        <v>0.01596231276668466</v>
       </c>
       <c r="D51" t="n">
-        <v>-0.02965811450799107</v>
+        <v>0.01544425588520481</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.004497842949371862</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="inlineStr">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
         <is>
           <t>Taurine</t>
         </is>
       </c>
-      <c r="B52" t="n">
-        <v>0.00982218308646675</v>
-      </c>
       <c r="C52" t="n">
-        <v>0.01234098105114076</v>
+        <v>0.0304273546482884</v>
       </c>
       <c r="D52" t="n">
-        <v>-0.1466667493774998</v>
+        <v>0.02734918519418263</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.0112653972845811</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="inlineStr">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
         <is>
           <t>Tyrosine</t>
         </is>
       </c>
-      <c r="B53" t="n">
-        <v>-0.000660503086104673</v>
-      </c>
       <c r="C53" t="n">
-        <v>3.956998382475485e-05</v>
+        <v>0.01919565384251291</v>
       </c>
       <c r="D53" t="n">
-        <v>-0.07944174049746792</v>
+        <v>0.02144942965486156</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.006267876736798137</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="inlineStr">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
         <is>
           <t>Urobilinogen</t>
         </is>
       </c>
-      <c r="B54" t="n">
-        <v>-0.005182693113950583</v>
-      </c>
       <c r="C54" t="n">
-        <v>0.01174733536981951</v>
+        <v>0.02556958720050915</v>
       </c>
       <c r="D54" t="n">
-        <v>-0.09144213206993079</v>
+        <v>0.02156235178421098</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.007815461347258178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>